<commit_message>
add new feature about scraping using username and get the data and statistics
</commit_message>
<xml_diff>
--- a/application/tweets.xlsx
+++ b/application/tweets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,963 +453,878 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Juanrafael Hernandez</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-04-28T22:00:01.000Z</t>
+          <t>2024-05-06T22:05:28.000Z</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>How to clone a GitHub repository and import it to Unity. On my youtube channel https://youtu.be/c3vM029a93k #gamedev #unity #blog #github</t>
+          <t xml:space="preserve"> No caption needed </t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Polkadot Leader</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-05-01T16:19:45.000Z</t>
+          <t>2024-05-06T22:05:30.000Z</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t xml:space="preserve">In the last 2 years #Polkadot has seen very impressive growth
-With the staggering volume of #GitHub commits and the relentless activity of developers, I anticipate this momentum to not only persist but to surge even further ahead #Bullish </t>
+          <t xml:space="preserve"> Last but not least</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vincent Otieno</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-04-28T08:56:34.000Z</t>
+          <t>2024-05-06T20:04:01.000Z</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Don't forget to leave a Sub on my YouTube Channel:
-Really Appreciated!!
-https://youtube.com/@kwargdevs
-[Tags: #softwaredeveloper #100DaysOfCode #python #github]</t>
+          <t xml:space="preserve"> More details: https://intermiamicf.co/MessiTOTM12</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Destiny Saturday</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2024-05-05T20:57:33.000Z</t>
+          <t>2024-05-06T20:04:02.000Z</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> What if you could get PAID for solving GitHub issues?
-Over the next 30 days, I'm building GitEarn, a game-changing software that rewards devs for solving issues directly within GitHub!
-Follow along as I build 
-@gitearn
- from  idea to launch 
-#GitEarn #GitHub #buildinpublic</t>
+          <t xml:space="preserve">Familia gracias por el apoyo esta noche </t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Pater Practicus</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2024-05-03T16:08:40.000Z</t>
+          <t>2024-05-06T20:04:03.000Z</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>I've been building up more content on my new website including a new section on  https://paterpracticus.com/downloads linking to   #GitHub repositories. Particularly handy will be the 3D print files for my call status indicator when I finish the follow-up to this: https://youtu.be/Ch0FHyCTUvo?si=mcSB_kNsH8CufrH…</t>
+          <t>Lluvia de goles en casa 
+Goal Celebration x 
+@CaptainMorganUS</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Opire</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>2024-04-28T15:42:53.000Z</t>
+          <t>2024-05-05T02:19:57.000Z</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Solve this issue and earn $1,000.00! 
-Details here: https://github.com/typeorm/typeorm/issues/3357… 
-#EarnWithOpire #Rewards #GitHub #OpenSource #Opire</t>
+          <t xml:space="preserve"> Highlights | Watch all the goals of the night here: https://intermiamicf.co/MIAvNYRBHLS</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aakash Web</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>2024-05-05T18:00:03.000Z</t>
+          <t>2024-05-05T01:59:25.000Z</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>You can also use "Git it write" plugin to blog in #WordPress from the comfort of your favorite desktop IDE
-Write your posts in #markdown format, push it to a #Github repository and voila your post is published in your website
-More information - https://wordpress.org/plugins/git-it-write/…
-#vscode</t>
+          <t xml:space="preserve">A NIGHT TO REMEMBER </t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Aniket</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2024-05-05T23:29:57.000Z</t>
+          <t>2024-05-05T01:57:44.000Z</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>think i’ve written at least 30,000 lines of code in the past few months and have no green dots to show for it  #github</t>
+          <t>90+6 | Goal for New York 
+#MIAvNYRB | 6-2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2024-05-04T19:47:16.000Z</t>
+          <t>2024-05-05T01:37:41.000Z</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>#GitHub stats are shaping up nicely…  https://github.com/cdaprod</t>
+          <t xml:space="preserve">Making history… AGAIN:  assists  goal tonight for the </t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gani Mendoza</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2024-05-04T00:02:30.000Z</t>
+          <t>2024-05-05T01:35:54.000Z</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Is #GitHub a worthy alternative to #JIRA?
-https://lightdash.com/blogpost/is-github-a-worthy-alternative-to-jira…</t>
+          <t>45’ | #PubSub x 
+@Publix
+IN: M. Rojas
+OUT: D. Ruiz 
+#MIAvNYRB 0-1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Sa Aaron</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2024-04-30T07:58:20.000Z</t>
+          <t>2024-05-05T01:32:09.000Z</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Checkout my new project - Litemail
-"A simple, lightweight, and fast email system built in PHP. Seamlessly send emails to other users, ensuring efficiency and ease of use."
-https://github.com/saaaron/Litemail…
-#100DaysOfCode #GitHub #php #webdeveloper #developer #tech</t>
+          <t>Here we go again! VAMOS! 
+Watch the 2nd half here: https://intermiamicf.co/MIAvNYRBstream</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Asjad Naqvi</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2024-05-02T14:35:09.000Z</t>
+          <t>2024-05-05T00:45:14.000Z</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>#Stata #splinefit is now upgraded from a random piece to code to a proper command. 
-The command is still in a very early phase so please open issues, enhancement requests etc on #GitHub:
-https://github.com/asjadnaqvi/stata-splinefit…</t>
+          <t>Down at the break. #VamosMiami</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rohan Shrivastava</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2024-04-30T17:45:34.000Z</t>
+          <t>2024-05-05T00:42:38.000Z</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Finally Made it. “Netflix Clone”
-With the help and guidance of 
-@codewithharry
- video on Youtube via Sigma Web Development Playlist.
-Source Code - https://bit.ly/44kE8Fe
-Check out the Project !! 
-#WebDevelopment #Connect #Tech #Follow #Netflix #Clone #Github #Html #CSS</t>
+          <t>29’ I Goal for New York.
+#MIAvNYRB 0-1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Vansh Chauhan</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2024-04-29T14:28:16.000Z</t>
+          <t>2024-05-05T00:28:11.000Z</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Celebrating My GitHub Contributions! 
-GitHub  https://lnkd.in/gTuQpvEx
- I've been actively contributing to open-source projects on GitHub. 
- I believe that consistent contributions drive innovation and foster collaboration.
-#GitHub #OpenSource #TechCommunity</t>
+          <t>We’re live from Chase Stadium 
+#MIAvNYRB | Tune in here: https://intermiamicf.co/MIAvNYRBstream</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>David Fowler</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2024-05-04T14:58:02.000Z</t>
+          <t>2024-05-05T00:10:37.000Z</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>2.9K  Thank you! 
-https://star-history.com/#dotnet/aspire&amp;Date…
-http://github.com/dotnet/aspire
-#starhistory #GitHub #OpenSource via 
-@StarHistoryHQ</t>
+          <t>Cada 31 minutos el juego cambia  Leo Messi conquista el Premio al Jugador del Mes de la 
+@MLS
+ en Abril tras 10 contribuciones de gol en 4 partidos.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Vicer Solutions</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2024-04-29T18:45:01.000Z</t>
+          <t>2024-05-04T23:44:26.000Z</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>See how a large Norwegian insurance company built a security-first application platform with the Microsoft developer platform. #coding #develop #apps #GitHub</t>
+          <t>Wishing you a very happy birthday DB</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Aahil, Thecr3ator</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2024-05-03T06:50:57.000Z</t>
+          <t>2024-05-02T23:53:07.000Z</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>NEW ARTICLE 
-This article will guide you through the process of checking out tags in Git, covering both local and remote tags and providing best practices for working with tags effectively. 
-#Git #GitHub</t>
+          <t>Flash to this incredible strike by Roby Taylor against NYRB!</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Pak Cyberbot</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2024-04-28T10:27:43.000Z</t>
+          <t>2024-05-02T21:57:26.000Z</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Doesn't it look like 
-@github
- 's mascot, the Octocat? 
-https://youtu.be/ARTZ_BGGhpE?si=QSSwe4jVNzsvqlzm&amp;t=103…
-#github #octocat #IF #mascot</t>
+          <t>A class apart!  Leo Messi takes home the 
+@MLS
+ Player of the Month award in April with an impressive 6 goals and 4 assists!  
+Details: https://intermiamicf.co/MessiAprilPOTM</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Multifverse</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2024-05-01T08:31:49.000Z</t>
+          <t>2024-05-02T21:00:00.000Z</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>GitHubが、AIを基盤とした統合開発環境（IDE）「Copilot Workspace」を発表しました。最近、次々と登場するコード生成AIに対応するため、新しい開発プラットフォームを提供し、開発者の利便性とアクセス性を大幅に強化する意図があります。https://x.gd/0lKcU #Copilot #GitHub #コード生成</t>
+          <t xml:space="preserve">Working towards #MIAvNYRB </t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Microsoft Thailand</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2024-05-01T03:02:01.000Z</t>
+          <t>2024-05-02T19:35:12.000Z</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Thailand has more than 900,000 developers on GitHub, growing 24% over the year.With GitHub Copilot,we’re increasing developer productivity by up to 55%,while helping developers stay in the flow and bringing the joy back to coding.
-#MSBuildAI #CEOVisit #MicrosoftThailand #GitHub</t>
+          <t xml:space="preserve">Así fue el primer gol del 'Pipa' Higuain  #MIAvNYRB </t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Michael Kaufmann</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2024-05-02T08:22:28.000Z</t>
+          <t>2024-05-02T15:16:42.000Z</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>My 4th book is now available: 
-@GitHub
- Actions Cookbook. It's a cookbook - so expect practical, hands-on recipes that will teach you all there is to know about GitHub Actions. 
-https://amazon.com/GitHub-Actions-Cookbook-streamlining-development/dp/1835468942…
-#GitHub #GitHubActions #Workflows #Automation #CICD</t>
+          <t>88’ | EL PISTOLEROOO 
+#NEvMIA | 1-4</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>RubyOnRails.BA</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>2024-05-05T12:00:25.000Z</t>
+          <t>2024-05-01T23:00:00.000Z</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Why Every User Without a Profile Picture on GitHub Was Yehuda Katz (from 17/03/2023) #ruby #rubyonrails #programming #github</t>
+          <t xml:space="preserve">Impacto inmediato de Benja! </t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Hemang Yadav</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2024-05-02T04:36:47.000Z</t>
+          <t>2024-04-28T01:30:49.000Z</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Hey #X Algorithm,
-Drop your #github profile below. Let's #connect &amp; #grow together. 
-Here's mine -</t>
+          <t>83’ | Cremaschi está de vuelta 
+#NEvMIA | 1-3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Orhun Parmaksız</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2024-05-02T20:17:45.000Z</t>
+          <t>2024-04-28T01:27:19.000Z</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>It's important to keep your pentest organized.
-I hope you find this useful 
-#Pentesting #Hacking #GitHub</t>
+          <t>74’ | #PubSub x  
+@Publix
+IN: B. Cremaschi
+OUT: J. Gressel
+IN: M. Rojas
+OUT: R. Taylor
+#NEvMIA 1-2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Ville Pakarinen</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2024-04-30T00:10:00.000Z</t>
+          <t>2024-04-28T01:26:16.000Z</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Git and GitHub Tutorial || Git Architecture || Git Crash Course || Professional Git
-☞ https://morioh.com/p/894cc1c0c3ca?f=5cb7d89d660c8335951ca454…
-#github #git #programming</t>
+          <t xml:space="preserve">Que bien se conocen! 
+Busi  Messi </t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Git and GitHub</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2024-04-29T02:09:00.000Z</t>
+          <t>2024-04-28T01:13:33.000Z</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Git And GitHub Full Course | Git And GitHub Tutorial For Beginners 
-☞ https://morioh.com/p/47c9ea1684d5?f=5cb7d89d660c8335951ca454…
-#git #github #javascript #python #developer</t>
+          <t>67’ | Segundo de Leo para darlo vuelta 
+#NEvMIA | 1-2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Okwudili O</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2024-05-03T05:56:03.000Z</t>
+          <t>2024-04-28T01:12:37.000Z</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>We Bring Our Thoughts to #Creativity 
-I'm thrilled to share my latest project, where I built a #fullstack burger app using #ReactNative and #Expo Go! 
-Scan Barcode and Free #Code on #GitHub
-https://bit.ly/4blZxQN 
- #MobileAppDevelopment  #OpenSource #TechInnovation</t>
+          <t>Gameday beats 
+Get ready for tomorrow’s match with Drake’s Hype by 
+@Heineken_US
+ playlist: https://intermiamicf.co/HypeByDrake</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>prod42net</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2024-04-27T20:09:00.000Z</t>
+          <t>2024-04-28T01:11:08.000Z</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Will GitHub Copilot Replace Flutter Developers?
-☞ https://morioh.com/p/38cd319d8021?f=5cb7d89d660c8335951ca454…
-#github #copilot #flutter #javascript #dart</t>
+          <t xml:space="preserve">A hattrick impossible to forget  #NEvMIA </t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Grand Panda</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2024-04-29T11:31:03.000Z</t>
+          <t>2024-04-26T22:00:00.000Z</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Learn how to push a local project to a remote Git repository with this comprehensive guide by Niladri Das. Also, discover how to prompt user input and store it in a JSON file using a Python project. #Git #Python #Programming #GitHub</t>
+          <t xml:space="preserve">The preparation continues </t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Vitalii Kapatsyna</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2024-04-29T18:30:05.000Z</t>
+          <t>2024-04-26T20:00:00.000Z</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Ready to supercharge your coding game? Copilot Workspace by GitHub offers a game-changing dev environment with AI assistance &amp; collaborative workflows. Say goodbye to coding struggles! #CopilotWorkspace #GitHub #CodingRevolution </t>
+          <t>Get ready to relive the dream!  Join us as we defend the #LeaguesCup title against Puebla on July 27 at Chase Stadium. Get your tickets now:  https://intermiamicf.co/TwitterLeaguesCupPuebla0727…</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>RemoteWLB</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2024-05-02T04:30:33.000Z</t>
+          <t>2024-04-26T19:20:05.000Z</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>"GitLab vs GitHub: Which is right for your project?  GitLab offers a complete DevOps solution with built-in CI/CD, while GitHub excels in version control. Dive into the comparison and make the right choice for your development needs. #GitLab #GitHub #D…</t>
+          <t>Away gameday incoming 
+Check out our Match Preview as we prepare to take on New England Revolution tomorrow at 7:30PM ET: https://intermiamicf.co/NEvMIAPreview</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Linux TLDR</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2024-04-29T16:07:35.000Z</t>
+          <t>2024-04-26T18:06:27.000Z</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Excited to dive into the world of AI-powered software engineering with Copilot Workspace by GitHub!  Can't wait to see how this game-changing tool will enhance our coding experience. #GitHub #CopilotWorkspace #AIprogramming #GameChanger:</t>
+          <t>Bienvenido al sueño, Matías! 
+We have signed Paraguayan national team midfielder Matías Rojas.
+ Details: https://intermiamicf.co/MatiasRojasSigning…</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Mohi.plena |</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2024-04-27T16:08:07.000Z</t>
+          <t>2024-04-26T18:00:00.000Z</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance the journey of "jolveragq/dutti-cli" with Opire! Your rewards can incentive collaboration and growth. Get started today: 
-https://github.com/jolveragq/dutti-cli…
-#Opire #OpenSource #dutti-cli #GitHub</t>
+          <t xml:space="preserve">50 assists from Suárez to Messi. What a dream duo!  </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Crypto News on Grafa</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2024-05-03T12:18:01.000Z</t>
+          <t>2024-04-23T20:07:59.000Z</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Are you looking for remote dev jobs?
-Look at this repo.
-YTML (You'll Thank Me Later)
-#remotework #remotejob #GitHub #SoftwareEngineer</t>
+          <t xml:space="preserve">Poetry in motion </t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>ITsAli.com</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2024-04-28T00:20:54.000Z</t>
+          <t>2024-04-22T22:00:01.000Z</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>"GitHub Copilot, the most widely adopted AI tool in history, suggests code, answers questions, refactors, and fixes issues. But be cautious of overreliance on automated suggestions to ensure code accuracy. Thanks, Abigael Wairimu! #GitHub #AI #Coding"</t>
+          <t>After their exceptional displays over the weekend, Lionel Messi and Sergio Busquets have been selected for the 
+@MLS
+ Team of the Week. Well done, guys! 
+Details: https://intermiamicf.co/MessiBusiTOTM</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Web Development</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2024-05-03T05:51:47.000Z</t>
+          <t>2024-04-22T19:58:29.000Z</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Tokei: Quickly Count Different Metrics in Your Codebase
-#Linux #Tokei #Programming #Coding #GitHub #DevOps</t>
+          <t>Injury Update x Baptist Health  
+The club has provided an injury update for midfielder Diego Gómez: https://intermiamicf.co/GomezUpdate</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>web3new.bnb</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2024-05-03T18:52:00.000Z</t>
+          <t>2024-04-22T18:50:04.000Z</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Enhance the journey of "jolveragq/gsap-scroll-test" with Opire! Your rewards can incentive collaboration and growth. Get started today: 
-https://github.com/jolveragq/gsap-scroll-test…
-#Opire #OpenSource #gsap-scroll-test #GitHub</t>
+          <t xml:space="preserve">Our Captain has been nominated for 
+@MLS
+Player of the Matchday! #VoteMessi </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Allwell</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2024-05-02T04:05:18.000Z</t>
+          <t>2024-04-22T17:43:54.000Z</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Just earned this exclusive Credential for my #GitHub contributions in 
-@aspecta_id
-'s #BuilderMatrix. Join now to discover your builder achievements and earn your very own #BuilderNFT! Check it out here:</t>
+          <t xml:space="preserve">Llegó el primer gol de Busi </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>·.¸¸.·♩♪♫ 𝙰𝚗𝚍𝚢 𝚆𝚞 ♫♪♩·.¸¸.·</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2024-04-27T09:20:40.000Z</t>
+          <t>2024-04-22T12:55:07.000Z</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Commit Frenzy : $CTC  - Developers committed 2.3X the rolling average code to Creditcoin this week, published 05/02/2024 #GitHub  
-@creditcoin</t>
+          <t>39 ' | GOOOOL DE BUSI 
+#MIAvNSH | 2-1</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Kourosh Hamdi</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2024-05-04T21:54:51.000Z</t>
+          <t>2024-04-21T00:25:39.000Z</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Just released version 2.0.0 of react-native-awesome-template! Simplify and enhance your React Native app development with pre-commit hooks, code linting, log cleanup, and more. Check it out on GitHub. #ReactNative #AppDevelopment #GitHub #CodingTips</t>
+          <t xml:space="preserve">Messi being Messi </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>_kri</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2024-05-01T16:14:06.000Z</t>
+          <t>2024-04-21T00:19:52.000Z</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Exportation of Git Repository Hosted on GitHub to AWS CodeCommit
-The seamless migration of a Git repository hosted on GitHub to AWS CodeCommit.
-https://techreport.us/2024/05/03/exportation-of-git-repository-hosted-on-github-to-aws-codecommit/…
-#aws #git #github #codecommit #blog</t>
+          <t xml:space="preserve">IT JUST HAD TO BE HIM </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Encora</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2024-05-03T15:58:15.000Z</t>
+          <t>2024-04-21T00:07:39.000Z</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Grand Real-time End-to-End DevOps CI/CD Project with Git, Jenkins, Docker, Kubernetes, and ArgoCD
-#jenkins #docker #github #kubernetes #docker</t>
+          <t>10' | GOL del 10 en el minuto 10
+#MIAvNSH | 1-1</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>ABP.IO</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2024-05-01T13:01:07.000Z</t>
+          <t>2024-04-20T23:55:43.000Z</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Just discovered this exclusive NFT for my #GitHub contributions in 
-@aspecta_id
-'s #BuilderMatrix. Join now to discover your builder achievements and earn your very own #BuilderNFT! Check it out here: https://aspecta.id/campaign/taiko?nft=12… </t>
+          <t>2' | Gol de Nashville 
+#MIAvNSH | 0-1</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Divyansh Jain</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2024-04-30T18:03:18.000Z</t>
+          <t>2024-04-20T23:51:38.000Z</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Learn how to setup a GitHub SSH connection by reading my article titled—How to Setup a GitHub SSH connection like a PRO.
-Check it out and let me know what you think.
-#github #ssh #git</t>
+          <t>We’re live from 
+@ChaseStadium
+#MIAvNSH  | Tune in here: https://intermiamicf.co/MIAvNSHstream</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Top 10 Trending GitHub Repos</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>2024-05-04T06:45:49.000Z</t>
+          <t>2024-04-20T23:47:22.000Z</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Last week, we released a highly automated pipeline to 
-1. publish package to npm registry
-2. build changelog (feature, bugfix ...)
-3. create #github release
-We will test it again if there is more room for improvement for coming up release (1.0.0-rc.8)</t>
+          <t xml:space="preserve">Not too long ago, Lucho scored this beauty  Tomorrow we meet again. #MIAvNSH </t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Crypto Topo</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>2024-05-03T15:48:08.000Z</t>
+          <t>2024-04-20T23:46:33.000Z</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Just discovered this exclusive NFT for my #GitHub contributions in 
-@aspecta_id
-'s #BuilderLaunchpad. Join now to discover your builder achievements and earn your very own #BuilderNFT! Check it out here:</t>
+          <t>Home match incoming 
+Check out our Match Preview as we prepare to take on Nashville tomorrow at 7:30 PM ET in our Ocean's Day match presented by 
+@FrachtGroup
+: https://intermiamicf.co/MIAvNSHpreview</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Ivan (이반) Porta</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>2024-05-02T14:29:08.000Z</t>
+          <t>2024-04-19T18:40:37.000Z</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Encora has achieved another specialization on Microsoft Azure: Specialization in DevOps with GitHub.  Congratulations to the entire team involved! 
-Read more: https://encora.com/news/encora-achieves-devops-excellence-with-github-microsoft-azure…
-#Azure #MicrosoftAzure #Encora #GitHub #Data #AI</t>
+          <t xml:space="preserve">Eyes on #MIAvNSH </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>NeowinFeed</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>2024-05-01T09:00:02.000Z</t>
+          <t>2024-04-19T18:00:01.000Z</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Ready to safeguard your digital assets? Brian Gorman 
-@blgorman
-'s #talk at #abpconf24, "Protecting Your Secrets using #Azure Key Vault, Azure App Configuration, #GitHub, and C# MVC", will transform your approach to secure coding. #csharp #MVC #dotnet 
-https://abp.io/conference/2024</t>
+          <t xml:space="preserve">Un sueño </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>damonemcrp</t>
+          <t>Inter Miami CF</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>2024-05-01T16:03:54.000Z</t>
+          <t>2024-04-18T21:17:43.000Z</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Exciting news! Introducing a flexible, responsive navbar for seamless navigation. Built with HTML, CSS, &amp; JavaScript, it ensures a smooth user experience on any device.
-Link : http://divyanshdj.github.io/navbar/
- #Navbar #HTML #CSS #JavaScript #WebDevelopment #UI #UserExperience #GitHub</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>WEBMAN</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>2024-05-03T13:38:48.000Z</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Top 10 Trending Repos  on #Github 
-1. pykan 
-Kolmogorov Arnold Networks 
-#Jupyter Notebook</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>灰黑度</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>2024-05-03T12:39:21.000Z</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Just discovered this exclusive NFT for my #GitHub contributions in 
-@aspecta_id
-'s #BuilderMatrix. Join now to discover your builder achievements and earn your very own #BuilderNFT! Check it out here:</t>
+          <t xml:space="preserve"> to this golazo against Nashville. #MIAvNSH </t>
         </is>
       </c>
     </row>

</xml_diff>